<commit_message>
Actualización formatos con identidad gráfica
</commit_message>
<xml_diff>
--- a/docs/formats/MISW-DA-Inception-CalculoVelocidad.xlsx
+++ b/docs/formats/MISW-DA-Inception-CalculoVelocidad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\mt2_procesos_guias_proyecto\docs\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B45CEF51-DCA9-43E3-8315-F431CC3059A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C0AC56-B9AC-412C-A13B-8A8DEBF39E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="975" windowWidth="28455" windowHeight="13980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instrucciones" sheetId="3" r:id="rId1"/>
@@ -361,6 +361,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -396,18 +408,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -437,16 +437,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>2425</xdr:rowOff>
+      <xdr:rowOff>24408</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1243C72E-5ECD-4C7E-A8B0-94FED2B4500B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7687326C-A2AC-4FFE-9598-19CDF0E35C5D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -469,7 +469,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7562850" cy="1755025"/>
+          <a:ext cx="7581900" cy="1777008"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -486,22 +486,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>1511885</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>16967</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
+        <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79852953-FCF6-4432-B7B7-20C33AD90914}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{967ADE40-80E3-4DCF-B7A2-C9EC94425759}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -523,8 +523,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9525" y="0"/>
-          <a:ext cx="6515100" cy="1511885"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6534150" cy="1531442"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -802,7 +802,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -819,11 +819,11 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -831,11 +831,11 @@
       <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
@@ -912,7 +912,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -928,116 +928,116 @@
       <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="29"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="17"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="30"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="30"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="30"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="30"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="18"/>
     </row>
     <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
-      <c r="D7" s="30"/>
+      <c r="D7" s="18"/>
     </row>
     <row r="8" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="30"/>
+      <c r="D8" s="18"/>
     </row>
     <row r="9" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="30"/>
+      <c r="D9" s="18"/>
     </row>
     <row r="10" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="30"/>
+      <c r="D10" s="18"/>
     </row>
     <row r="11" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="30"/>
+      <c r="D11" s="18"/>
     </row>
     <row r="12" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="30"/>
+      <c r="D12" s="18"/>
     </row>
     <row r="13" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="30"/>
+      <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="30"/>
+      <c r="D14" s="18"/>
     </row>
     <row r="15" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="25">
         <f>B6*B5*B4-(SUM(C7:C13))</f>
         <v>0</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="30"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="17" t="e">
+      <c r="B16" s="21" t="e">
         <f>B15*PHU_HBUBase/Horas_HUBase</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="31"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1071,56 +1071,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
     </row>
     <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="25">
         <f>SUM(C10:C30)</f>
         <v>0</v>
       </c>
-      <c r="C6" s="21"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1132,7 +1132,7 @@
       <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="28"/>
+      <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1296,6 +1296,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003971913424ECAE4E805D1BC6E6D9BC3C" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="2ba7d757ff0ecd0ad482a876eccc7a5d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4d58fc9-363e-42d3-93a3-0f0e39d2b62b" xmlns:ns3="0e733887-b47c-44a5-a322-08148880beac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c1f5668d3ea10092d56e455a4b03d3b4" ns2:_="" ns3:_="">
     <xsd:import namespace="a4d58fc9-363e-42d3-93a3-0f0e39d2b62b"/>
@@ -1506,12 +1512,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1522,6 +1522,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{798442E3-493D-49EE-9C69-501BF1ADA746}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB435DA9-82E7-4EA9-AC5D-283D86B38EC5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1540,15 +1549,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{798442E3-493D-49EE-9C69-501BF1ADA746}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33E1B388-BAD6-4BFE-80EC-AC0C7F4AA802}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Se agrega nueva ficha de lectura para retrospectivas
</commit_message>
<xml_diff>
--- a/docs/formats/MISW-DA-Inception-CalculoVelocidad.xlsx
+++ b/docs/formats/MISW-DA-Inception-CalculoVelocidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\mt2_procesos_guias_proyecto\docs\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C0AC56-B9AC-412C-A13B-8A8DEBF39E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C32E3060-0F4A-4340-94E1-34B4CB2DA6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="Horas_HUBase">EstimaciónHUBase!$B$6</definedName>
     <definedName name="PHU_HBUBase">EstimaciónHUBase!$B$5</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Equipo</t>
   </si>
@@ -51,78 +51,81 @@
     <t>Número del equipo</t>
   </si>
   <si>
-    <t>Nº Horas por Semana</t>
+    <t>Tareas transversales al proyecto</t>
+  </si>
+  <si>
+    <t>Detalle de Velocidad del Sprint Equipo</t>
+  </si>
+  <si>
+    <t>Total Horas Asignadas para el Sprint</t>
+  </si>
+  <si>
+    <t>Velocidad del Sprint</t>
+  </si>
+  <si>
+    <t>Historia de Usuario Base</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Narrativa</t>
+  </si>
+  <si>
+    <t>Puntos de Historia de Usuario asignados a la historia</t>
+  </si>
+  <si>
+    <t>Actividades</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>1. Digite la información de la estimación de la historia base en la hoja EstimaciónHUBase</t>
+  </si>
+  <si>
+    <t>2. Digite la siguiente información en la hoja VelocidadEquipo</t>
+  </si>
+  <si>
+    <t>3. Verifique el resultado del cálculo de velocidad en la celda Velocidad del sprint.</t>
+  </si>
+  <si>
+    <t>Número de semanas del sprint.</t>
+  </si>
+  <si>
+    <t>Cantidad de miembros en el equipo.</t>
+  </si>
+  <si>
+    <t>Realice los siguientes pasos para calcular la velocidad del equipo:</t>
+  </si>
+  <si>
+    <t>N.º Horas por Semana</t>
+  </si>
+  <si>
+    <t>N.º Semanas</t>
+  </si>
+  <si>
+    <t>N.º de Desarrolladores</t>
+  </si>
+  <si>
+    <t>Consignen la lista de actividades transversales que se deben realizar durante el sprint y los tiempos estimados para las mismas. Una tarea transversal es una tarea que se debe realizar y no se hace para una historia particular. Un ejemplo de tarea transversal es la actividad de grooming de historias.</t>
+  </si>
+  <si>
+    <t>N.º Horas por semana</t>
+  </si>
+  <si>
+    <t>Título</t>
+  </si>
+  <si>
+    <t>Sumatoria de horas</t>
+  </si>
+  <si>
+    <t>Estimación de horas</t>
   </si>
   <si>
     <t>Horas por semana dedicadas al proyecto por cada miembro. Tener en cuenta que:
 - La dedicación esperada por semana para el curso según el número de créditos es de 12 horas.
-- Se espera que de estas 12 horas los estudiantes dediquen entre 3 y 4 horas a actividades de aprendizaje y  que no  hacen parte del proyecto.</t>
-  </si>
-  <si>
-    <t>Nº Semanas</t>
-  </si>
-  <si>
-    <t>Nº de Desarrolladores</t>
-  </si>
-  <si>
-    <t>Tareas transversales al proyecto</t>
-  </si>
-  <si>
-    <t>Consignen la lista de actividades transversales que se deben realizar durantes el sprint y los tiempos estimados para las mismas. Una tarea transversal es una tarea que se debe realizar y no se hace para una historia particular. Un ejemplo de tarea transversal es la actividad de grooming de historias.</t>
-  </si>
-  <si>
-    <t>Detalle de Velocidad del Sprint Equipo</t>
-  </si>
-  <si>
-    <t>Total Horas Asignadas para el Sprint</t>
-  </si>
-  <si>
-    <t>Velocidad del Sprint</t>
-  </si>
-  <si>
-    <t>Historia de Usuario Base</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Titulo</t>
-  </si>
-  <si>
-    <t>Narrativa</t>
-  </si>
-  <si>
-    <t>Puntos de Historia de Usuario asignados a la historia</t>
-  </si>
-  <si>
-    <t>Sumatoria de Horas</t>
-  </si>
-  <si>
-    <t>Actividades</t>
-  </si>
-  <si>
-    <t>Descripción</t>
-  </si>
-  <si>
-    <t>Estimación de Horas</t>
-  </si>
-  <si>
-    <t>1. Digite la información de la estimación de la historia base en la hoja EstimaciónHUBase</t>
-  </si>
-  <si>
-    <t>2. Digite la siguiente información en la hoja VelocidadEquipo</t>
-  </si>
-  <si>
-    <t>3. Verifique el resultado del cálculo de velocidad en la celda Velocidad del sprint.</t>
-  </si>
-  <si>
-    <t>Número de semanas del sprint.</t>
-  </si>
-  <si>
-    <t>Cantidad de miembros en el equipo.</t>
-  </si>
-  <si>
-    <t>Realice los siguientes pasos para calcular la velocidad del equipo:</t>
+- Se espera que los estudiantes dediquen entre 3 y 4 horas a actividades de aprendizaje que no hacen parte del proyecto.</t>
   </si>
 </sst>
 </file>
@@ -431,22 +434,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>24408</xdr:rowOff>
+      <xdr:rowOff>15478</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7687326C-A2AC-4FFE-9598-19CDF0E35C5D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7990921-475E-498E-9354-AC2707012322}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -468,8 +471,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="7581900" cy="1777008"/>
+          <a:off x="19050" y="0"/>
+          <a:ext cx="7543800" cy="1768078"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -486,22 +489,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>16967</xdr:rowOff>
+      <xdr:rowOff>12501</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{967ADE40-80E3-4DCF-B7A2-C9EC94425759}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F1A4878-2E62-40CC-AE92-93DB21F3D664}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -523,8 +526,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="6534150" cy="1531442"/>
+          <a:off x="9525" y="0"/>
+          <a:ext cx="6515100" cy="1526976"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -802,7 +805,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -815,12 +818,12 @@
     <row r="1" spans="1:8" ht="138" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
@@ -832,7 +835,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
@@ -862,39 +865,39 @@
     </row>
     <row r="9" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -912,7 +915,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -929,7 +932,7 @@
     </row>
     <row r="2" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -945,7 +948,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -953,7 +956,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B5" s="25"/>
       <c r="C5" s="25"/>
@@ -961,7 +964,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B6" s="27"/>
       <c r="C6" s="28"/>
@@ -969,7 +972,7 @@
     </row>
     <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -1019,7 +1022,7 @@
     </row>
     <row r="15" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B15" s="25">
         <f>B6*B5*B4-(SUM(C7:C13))</f>
@@ -1030,7 +1033,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B16" s="21" t="e">
         <f>B15*PHU_HBUBase/Horas_HUBase</f>
@@ -1060,7 +1063,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1072,42 +1075,42 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B3" s="31"/>
       <c r="C3" s="31"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
     </row>
     <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B5" s="25"/>
       <c r="C5" s="25"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B6" s="25">
         <f>SUM(C10:C30)</f>
@@ -1117,20 +1120,20 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E9" s="16"/>
     </row>
@@ -1296,16 +1299,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003971913424ECAE4E805D1BC6E6D9BC3C" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="2ba7d757ff0ecd0ad482a876eccc7a5d">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4d58fc9-363e-42d3-93a3-0f0e39d2b62b" xmlns:ns3="0e733887-b47c-44a5-a322-08148880beac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c1f5668d3ea10092d56e455a4b03d3b4" ns2:_="" ns3:_="">
-    <xsd:import namespace="a4d58fc9-363e-42d3-93a3-0f0e39d2b62b"/>
-    <xsd:import namespace="0e733887-b47c-44a5-a322-08148880beac"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A819456F60CD2C48BCA8728434F1A741" ma:contentTypeVersion="6" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="3984a728b3e371fe645f30aafdd6dc97">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="34b779b8-fc51-4034-b286-8b23b89d0ca8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="258f7d7880366169d1bca51c729a44f9" ns2:_="">
+    <xsd:import namespace="34b779b8-fc51-4034-b286-8b23b89d0ca8"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -1314,15 +1310,10 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1330,7 +1321,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a4d58fc9-363e-42d3-93a3-0f0e39d2b62b" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="34b779b8-fc51-4034-b286-8b23b89d0ca8" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -1343,73 +1334,26 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="17" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="18" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="0e733887-b47c-44a5-a322-08148880beac" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="11" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="12" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1512,6 +1456,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1522,29 +1472,35 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{798442E3-493D-49EE-9C69-501BF1ADA746}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB435DA9-82E7-4EA9-AC5D-283D86B38EC5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97855BBE-7BBF-49E8-B49C-AFC8715E199E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a4d58fc9-363e-42d3-93a3-0f0e39d2b62b"/>
-    <ds:schemaRef ds:uri="0e733887-b47c-44a5-a322-08148880beac"/>
+    <ds:schemaRef ds:uri="34b779b8-fc51-4034-b286-8b23b89d0ca8"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{798442E3-493D-49EE-9C69-501BF1ADA746}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="34b779b8-fc51-4034-b286-8b23b89d0ca8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>